<commit_message>
Condensing of scripts and better logging
</commit_message>
<xml_diff>
--- a/Sample_Prep_Helper_Template.xlsx
+++ b/Sample_Prep_Helper_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sys_op\methods\Development\AMEX_Template_BD\USCS-Sample-Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF74B26E-B8DD-45E1-A042-3687FEEBBA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E0F29F-916E-4BCA-A8FF-B2C5B99797C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{FBE6EFD9-31E1-4B03-A058-28FE4160739B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{FBE6EFD9-31E1-4B03-A058-28FE4160739B}"/>
   </bookViews>
   <sheets>
     <sheet name="Augment_Specs" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="447">
   <si>
     <t>Card Name</t>
   </si>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">Total Sample needed </t>
   </si>
   <si>
-    <t>naw_cell_code</t>
-  </si>
-  <si>
     <t>weighting_segment</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>sp_code</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>No Code --- Not in a DMA</t>
   </si>
   <si>
@@ -1357,27 +1351,12 @@
     <t>Valid_DMA</t>
   </si>
   <si>
-    <t>CELL14</t>
-  </si>
-  <si>
     <t>Any Spend</t>
   </si>
   <si>
-    <t>CELL18</t>
-  </si>
-  <si>
-    <t>CELL21</t>
-  </si>
-  <si>
     <t>&gt;$0</t>
   </si>
   <si>
-    <t>CELL22</t>
-  </si>
-  <si>
-    <t>CELL35</t>
-  </si>
-  <si>
     <t>X2</t>
   </si>
   <si>
@@ -1385,6 +1364,30 @@
   </si>
   <si>
     <t>X1</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>cell_code</t>
+  </si>
+  <si>
+    <t>CNCE14</t>
+  </si>
+  <si>
+    <t>CNDP22</t>
+  </si>
+  <si>
+    <t>CNHH21</t>
+  </si>
+  <si>
+    <t>CNPL18</t>
+  </si>
+  <si>
+    <t>CNPR35</t>
   </si>
 </sst>
 </file>
@@ -8305,7 +8308,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8318,7 +8321,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>441</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -8332,18 +8335,18 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="B2" s="3">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -8352,12 +8355,12 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -8366,12 +8369,12 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -8380,12 +8383,12 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -8394,7 +8397,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -8408,7 +8411,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8624,7 +8627,7 @@
   <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8636,18 +8639,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>440</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>439</v>
       </c>
       <c r="C1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -8655,10 +8658,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -8666,10 +8669,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>501</v>
@@ -8677,10 +8680,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>502</v>
@@ -8688,10 +8691,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>503</v>
@@ -8699,10 +8702,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>504</v>
@@ -8710,10 +8713,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>505</v>
@@ -8721,10 +8724,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>506</v>
@@ -8732,10 +8735,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>507</v>
@@ -8743,10 +8746,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>508</v>
@@ -8754,10 +8757,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>509</v>
@@ -8765,10 +8768,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>510</v>
@@ -8776,10 +8779,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <v>511</v>
@@ -8787,10 +8790,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <v>512</v>
@@ -8798,10 +8801,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16">
         <v>513</v>
@@ -8809,10 +8812,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>514</v>
@@ -8820,10 +8823,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>515</v>
@@ -8831,10 +8834,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>516</v>
@@ -8842,10 +8845,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>517</v>
@@ -8853,10 +8856,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21">
         <v>518</v>
@@ -8864,10 +8867,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22">
         <v>519</v>
@@ -8875,10 +8878,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23">
         <v>520</v>
@@ -8886,10 +8889,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24">
         <v>521</v>
@@ -8897,10 +8900,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25">
         <v>522</v>
@@ -8908,10 +8911,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26">
         <v>523</v>
@@ -8919,10 +8922,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>524</v>
@@ -8930,10 +8933,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28">
         <v>525</v>
@@ -8941,10 +8944,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29">
         <v>526</v>
@@ -8952,10 +8955,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C30">
         <v>527</v>
@@ -8963,10 +8966,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C31">
         <v>528</v>
@@ -8974,10 +8977,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C32">
         <v>529</v>
@@ -8985,10 +8988,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C33">
         <v>530</v>
@@ -8996,10 +8999,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C34">
         <v>531</v>
@@ -9007,10 +9010,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C35">
         <v>532</v>
@@ -9018,10 +9021,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C36">
         <v>533</v>
@@ -9029,10 +9032,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C37">
         <v>534</v>
@@ -9040,10 +9043,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C38">
         <v>535</v>
@@ -9051,10 +9054,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>536</v>
@@ -9062,10 +9065,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40">
         <v>537</v>
@@ -9073,10 +9076,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41">
         <v>538</v>
@@ -9084,10 +9087,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C42">
         <v>539</v>
@@ -9095,10 +9098,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C43">
         <v>540</v>
@@ -9106,10 +9109,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C44">
         <v>541</v>
@@ -9117,10 +9120,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45">
         <v>542</v>
@@ -9128,10 +9131,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C46">
         <v>543</v>
@@ -9139,10 +9142,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C47">
         <v>544</v>
@@ -9150,10 +9153,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C48">
         <v>545</v>
@@ -9161,10 +9164,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C49">
         <v>546</v>
@@ -9172,10 +9175,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C50">
         <v>547</v>
@@ -9183,10 +9186,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C51">
         <v>548</v>
@@ -9194,10 +9197,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C52">
         <v>549</v>
@@ -9205,10 +9208,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C53">
         <v>550</v>
@@ -9216,10 +9219,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C54">
         <v>551</v>
@@ -9227,10 +9230,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B55" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C55">
         <v>552</v>
@@ -9238,10 +9241,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C56">
         <v>553</v>
@@ -9249,10 +9252,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C57">
         <v>554</v>
@@ -9260,10 +9263,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C58">
         <v>555</v>
@@ -9271,10 +9274,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C59">
         <v>556</v>
@@ -9282,10 +9285,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B60" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C60">
         <v>557</v>
@@ -9293,10 +9296,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C61">
         <v>558</v>
@@ -9304,10 +9307,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C62">
         <v>559</v>
@@ -9315,10 +9318,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C63">
         <v>560</v>
@@ -9326,10 +9329,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C64">
         <v>561</v>
@@ -9337,10 +9340,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C65">
         <v>563</v>
@@ -9348,10 +9351,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C66">
         <v>564</v>
@@ -9359,10 +9362,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C67">
         <v>565</v>
@@ -9370,10 +9373,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C68">
         <v>566</v>
@@ -9381,10 +9384,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C69">
         <v>567</v>
@@ -9392,10 +9395,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C70">
         <v>569</v>
@@ -9403,10 +9406,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B71" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C71">
         <v>570</v>
@@ -9414,10 +9417,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C72">
         <v>571</v>
@@ -9425,10 +9428,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C73">
         <v>573</v>
@@ -9436,10 +9439,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C74">
         <v>574</v>
@@ -9447,10 +9450,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C75">
         <v>575</v>
@@ -9458,10 +9461,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B76" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C76">
         <v>576</v>
@@ -9469,10 +9472,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B77" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C77">
         <v>577</v>
@@ -9480,10 +9483,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B78" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C78">
         <v>581</v>
@@ -9491,10 +9494,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B79" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C79">
         <v>582</v>
@@ -9502,10 +9505,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B80" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C80">
         <v>583</v>
@@ -9513,10 +9516,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B81" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C81">
         <v>584</v>
@@ -9524,10 +9527,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B82" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C82">
         <v>588</v>
@@ -9535,10 +9538,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B83" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C83">
         <v>592</v>
@@ -9546,10 +9549,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B84" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C84">
         <v>596</v>
@@ -9557,10 +9560,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C85">
         <v>597</v>
@@ -9568,10 +9571,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B86" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C86">
         <v>598</v>
@@ -9579,10 +9582,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B87" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C87">
         <v>600</v>
@@ -9590,10 +9593,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B88" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C88">
         <v>602</v>
@@ -9601,10 +9604,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B89" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C89">
         <v>603</v>
@@ -9612,10 +9615,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B90" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C90">
         <v>604</v>
@@ -9623,10 +9626,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B91" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C91">
         <v>605</v>
@@ -9634,10 +9637,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B92" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C92">
         <v>606</v>
@@ -9645,10 +9648,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B93" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C93">
         <v>609</v>
@@ -9656,10 +9659,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B94" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C94">
         <v>610</v>
@@ -9667,10 +9670,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B95" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C95">
         <v>611</v>
@@ -9678,10 +9681,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B96" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C96">
         <v>612</v>
@@ -9689,10 +9692,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B97" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C97">
         <v>613</v>
@@ -9700,10 +9703,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B98" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C98">
         <v>616</v>
@@ -9711,10 +9714,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B99" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C99">
         <v>617</v>
@@ -9722,10 +9725,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B100" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C100">
         <v>618</v>
@@ -9733,10 +9736,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B101" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C101">
         <v>619</v>
@@ -9744,10 +9747,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B102" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C102">
         <v>622</v>
@@ -9755,10 +9758,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B103" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C103">
         <v>623</v>
@@ -9766,10 +9769,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B104" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C104">
         <v>624</v>
@@ -9777,10 +9780,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B105" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C105">
         <v>625</v>
@@ -9788,10 +9791,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B106" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C106">
         <v>626</v>
@@ -9799,10 +9802,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B107" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C107">
         <v>627</v>
@@ -9810,10 +9813,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B108" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C108">
         <v>628</v>
@@ -9821,10 +9824,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B109" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C109">
         <v>630</v>
@@ -9832,10 +9835,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B110" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C110">
         <v>631</v>
@@ -9843,10 +9846,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B111" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C111">
         <v>632</v>
@@ -9854,10 +9857,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B112" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C112">
         <v>633</v>
@@ -9865,10 +9868,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B113" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C113">
         <v>634</v>
@@ -9876,10 +9879,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B114" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C114">
         <v>635</v>
@@ -9887,10 +9890,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B115" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C115">
         <v>636</v>
@@ -9898,10 +9901,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B116" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C116">
         <v>637</v>
@@ -9909,10 +9912,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B117" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C117">
         <v>638</v>
@@ -9920,10 +9923,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B118" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C118">
         <v>639</v>
@@ -9931,10 +9934,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B119" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C119">
         <v>640</v>
@@ -9942,10 +9945,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B120" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C120">
         <v>641</v>
@@ -9953,10 +9956,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B121" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C121">
         <v>642</v>
@@ -9964,10 +9967,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B122" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C122">
         <v>643</v>
@@ -9975,10 +9978,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B123" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C123">
         <v>644</v>
@@ -9986,10 +9989,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B124" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C124">
         <v>647</v>
@@ -9997,10 +10000,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B125" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C125">
         <v>648</v>
@@ -10008,10 +10011,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B126" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C126">
         <v>649</v>
@@ -10019,10 +10022,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B127" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C127">
         <v>650</v>
@@ -10030,10 +10033,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B128" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C128">
         <v>651</v>
@@ -10041,10 +10044,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B129" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C129">
         <v>652</v>
@@ -10052,10 +10055,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B130" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C130">
         <v>656</v>
@@ -10063,10 +10066,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B131" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C131">
         <v>657</v>
@@ -10074,10 +10077,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B132" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C132">
         <v>658</v>
@@ -10085,10 +10088,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B133" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C133">
         <v>659</v>
@@ -10096,10 +10099,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B134" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C134">
         <v>661</v>
@@ -10107,10 +10110,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B135" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C135">
         <v>662</v>
@@ -10118,10 +10121,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B136" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C136">
         <v>669</v>
@@ -10129,10 +10132,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B137" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C137">
         <v>670</v>
@@ -10140,10 +10143,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B138" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C138">
         <v>671</v>
@@ -10151,10 +10154,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B139" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C139">
         <v>673</v>
@@ -10162,10 +10165,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B140" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C140">
         <v>675</v>
@@ -10173,10 +10176,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B141" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C141">
         <v>676</v>
@@ -10184,10 +10187,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B142" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C142">
         <v>678</v>
@@ -10195,10 +10198,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B143" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C143">
         <v>679</v>
@@ -10206,10 +10209,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B144" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C144">
         <v>682</v>
@@ -10217,10 +10220,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B145" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C145">
         <v>686</v>
@@ -10228,10 +10231,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B146" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C146">
         <v>687</v>
@@ -10239,10 +10242,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B147" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C147">
         <v>691</v>
@@ -10250,10 +10253,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B148" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C148">
         <v>692</v>
@@ -10261,10 +10264,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B149" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C149">
         <v>693</v>
@@ -10272,10 +10275,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B150" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C150">
         <v>698</v>
@@ -10283,10 +10286,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B151" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C151">
         <v>702</v>
@@ -10294,10 +10297,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B152" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C152">
         <v>705</v>
@@ -10305,10 +10308,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B153" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C153">
         <v>709</v>
@@ -10316,10 +10319,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B154" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C154">
         <v>710</v>
@@ -10327,10 +10330,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B155" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C155">
         <v>711</v>
@@ -10338,10 +10341,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B156" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C156">
         <v>716</v>
@@ -10349,10 +10352,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B157" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C157">
         <v>717</v>
@@ -10360,10 +10363,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B158" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C158">
         <v>718</v>
@@ -10371,10 +10374,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B159" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C159">
         <v>722</v>
@@ -10382,10 +10385,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B160" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C160">
         <v>724</v>
@@ -10393,10 +10396,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B161" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C161">
         <v>725</v>
@@ -10404,10 +10407,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B162" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C162">
         <v>734</v>
@@ -10415,10 +10418,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B163" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C163">
         <v>736</v>
@@ -10426,10 +10429,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B164" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C164">
         <v>737</v>
@@ -10437,10 +10440,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B165" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C165">
         <v>740</v>
@@ -10448,10 +10451,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B166" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C166">
         <v>743</v>
@@ -10459,10 +10462,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B167" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C167">
         <v>744</v>
@@ -10470,10 +10473,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B168" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C168">
         <v>745</v>
@@ -10481,10 +10484,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B169" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C169">
         <v>746</v>
@@ -10492,10 +10495,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B170" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C170">
         <v>747</v>
@@ -10503,10 +10506,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B171" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C171">
         <v>749</v>
@@ -10514,10 +10517,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B172" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C172">
         <v>751</v>
@@ -10525,10 +10528,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B173" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C173">
         <v>752</v>
@@ -10536,10 +10539,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B174" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C174">
         <v>753</v>
@@ -10547,10 +10550,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B175" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C175">
         <v>754</v>
@@ -10558,10 +10561,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B176" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C176">
         <v>755</v>
@@ -10569,10 +10572,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B177" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C177">
         <v>756</v>
@@ -10580,10 +10583,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B178" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C178">
         <v>757</v>
@@ -10591,10 +10594,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B179" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C179">
         <v>758</v>
@@ -10602,10 +10605,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B180" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C180">
         <v>759</v>
@@ -10613,10 +10616,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B181" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C181">
         <v>760</v>
@@ -10624,10 +10627,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B182" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C182">
         <v>762</v>
@@ -10635,10 +10638,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B183" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C183">
         <v>764</v>
@@ -10646,10 +10649,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B184" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C184">
         <v>765</v>
@@ -10657,10 +10660,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B185" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C185">
         <v>766</v>
@@ -10668,10 +10671,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B186" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C186">
         <v>767</v>
@@ -10679,10 +10682,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B187" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C187">
         <v>770</v>
@@ -10690,10 +10693,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B188" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C188">
         <v>771</v>
@@ -10701,10 +10704,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B189" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C189">
         <v>773</v>
@@ -10712,10 +10715,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B190" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C190">
         <v>789</v>
@@ -10723,10 +10726,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B191" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C191">
         <v>790</v>
@@ -10734,10 +10737,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B192" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C192">
         <v>798</v>
@@ -10745,10 +10748,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B193" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C193">
         <v>800</v>
@@ -10756,10 +10759,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B194" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C194">
         <v>801</v>
@@ -10767,10 +10770,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B195" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C195">
         <v>802</v>
@@ -10778,10 +10781,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B196" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C196">
         <v>803</v>
@@ -10789,10 +10792,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B197" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C197">
         <v>804</v>
@@ -10800,10 +10803,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B198" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C198">
         <v>807</v>
@@ -10811,10 +10814,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B199" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C199">
         <v>810</v>
@@ -10822,10 +10825,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B200" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C200">
         <v>811</v>
@@ -10833,10 +10836,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B201" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C201">
         <v>813</v>
@@ -10844,10 +10847,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B202" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C202">
         <v>819</v>
@@ -10855,10 +10858,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B203" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C203">
         <v>820</v>
@@ -10866,10 +10869,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B204" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C204">
         <v>821</v>
@@ -10877,10 +10880,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B205" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C205">
         <v>825</v>
@@ -10888,10 +10891,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B206" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C206">
         <v>828</v>
@@ -10899,10 +10902,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B207" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C207">
         <v>839</v>
@@ -10910,10 +10913,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B208" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C208">
         <v>855</v>
@@ -10921,10 +10924,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B209" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C209">
         <v>862</v>
@@ -10932,10 +10935,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B210" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C210">
         <v>866</v>
@@ -10943,10 +10946,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B211" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C211">
         <v>868</v>
@@ -10954,10 +10957,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B212" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C212">
         <v>881</v>
@@ -10965,10 +10968,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B213" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C213">
         <v>980</v>
@@ -10984,7 +10987,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11000,28 +11003,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="E1" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="F1" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>